<commit_message>
Add: WriteDB & Test Files
</commit_message>
<xml_diff>
--- a/Utilities/Datasets/Testing/test_xlsx.xlsx
+++ b/Utilities/Datasets/Testing/test_xlsx.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,198 +436,63 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Column_1</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Column_2</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Column_3</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Column_4</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Column_5</t>
+          <t>City</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>21</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>90</v>
-      </c>
-      <c r="C2" t="n">
-        <v>66</v>
-      </c>
-      <c r="D2" t="n">
-        <v>47</v>
-      </c>
-      <c r="E2" t="n">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>78</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
       </c>
       <c r="B3" t="n">
-        <v>18</v>
-      </c>
-      <c r="C3" t="n">
-        <v>60</v>
-      </c>
-      <c r="D3" t="n">
-        <v>69</v>
-      </c>
-      <c r="E3" t="n">
-        <v>99</v>
+        <v>30</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>65</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Charlie</t>
+        </is>
       </c>
       <c r="B4" t="n">
-        <v>66</v>
-      </c>
-      <c r="C4" t="n">
-        <v>95</v>
-      </c>
-      <c r="D4" t="n">
-        <v>92</v>
-      </c>
-      <c r="E4" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>16</v>
-      </c>
-      <c r="B5" t="n">
-        <v>9</v>
-      </c>
-      <c r="C5" t="n">
-        <v>75</v>
-      </c>
-      <c r="D5" t="n">
-        <v>29</v>
-      </c>
-      <c r="E5" t="n">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>81</v>
-      </c>
-      <c r="B6" t="n">
-        <v>9</v>
-      </c>
-      <c r="C6" t="n">
-        <v>76</v>
-      </c>
-      <c r="D6" t="n">
-        <v>93</v>
-      </c>
-      <c r="E6" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>40</v>
-      </c>
-      <c r="B7" t="n">
-        <v>63</v>
-      </c>
-      <c r="C7" t="n">
-        <v>75</v>
-      </c>
-      <c r="D7" t="n">
-        <v>54</v>
-      </c>
-      <c r="E7" t="n">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>28</v>
-      </c>
-      <c r="B8" t="n">
-        <v>76</v>
-      </c>
-      <c r="C8" t="n">
-        <v>24</v>
-      </c>
-      <c r="D8" t="n">
-        <v>64</v>
-      </c>
-      <c r="E8" t="n">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>67</v>
-      </c>
-      <c r="B9" t="n">
-        <v>16</v>
-      </c>
-      <c r="C9" t="n">
-        <v>10</v>
-      </c>
-      <c r="D9" t="n">
-        <v>33</v>
-      </c>
-      <c r="E9" t="n">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>33</v>
-      </c>
-      <c r="B10" t="n">
-        <v>26</v>
-      </c>
-      <c r="C10" t="n">
-        <v>72</v>
-      </c>
-      <c r="D10" t="n">
-        <v>95</v>
-      </c>
-      <c r="E10" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>72</v>
-      </c>
-      <c r="B11" t="n">
-        <v>63</v>
-      </c>
-      <c r="C11" t="n">
-        <v>83</v>
-      </c>
-      <c r="D11" t="n">
-        <v>14</v>
-      </c>
-      <c r="E11" t="n">
-        <v>31</v>
+        <v>22</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Chicago</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>